<commit_message>
Reprocess D2893, Edi06 and Edi09
</commit_message>
<xml_diff>
--- a/data/processed/basaltic_glasses/calczaf_files/D2893/calczaf_outputs.xlsx
+++ b/data/processed/basaltic_glasses/calczaf_files/D2893/calczaf_outputs.xlsx
@@ -5231,13 +5231,13 @@
         <v>0.349</v>
       </c>
       <c r="C10">
+        <v>0.349</v>
+      </c>
+      <c r="D10">
+        <v>0.348</v>
+      </c>
+      <c r="E10">
         <v>0.35</v>
-      </c>
-      <c r="D10">
-        <v>0.349</v>
-      </c>
-      <c r="E10">
-        <v>0.351</v>
       </c>
       <c r="F10">
         <v>0.35</v>
@@ -5246,10 +5246,10 @@
         <v>0.353</v>
       </c>
       <c r="H10">
-        <v>0.35</v>
+        <v>0.349</v>
       </c>
       <c r="I10">
-        <v>0.349</v>
+        <v>0.348</v>
       </c>
       <c r="J10">
         <v>0.351</v>
@@ -5258,28 +5258,28 @@
         <v>0.351</v>
       </c>
       <c r="L10">
+        <v>0.348</v>
+      </c>
+      <c r="M10">
+        <v>0.351</v>
+      </c>
+      <c r="N10">
         <v>0.349</v>
       </c>
-      <c r="M10">
-        <v>0.352</v>
-      </c>
-      <c r="N10">
-        <v>0.35</v>
-      </c>
       <c r="O10">
-        <v>0.35</v>
+        <v>0.349</v>
       </c>
       <c r="P10">
         <v>0.35</v>
       </c>
       <c r="Q10">
-        <v>0.351</v>
+        <v>0.35</v>
       </c>
       <c r="R10">
         <v>0.351</v>
       </c>
       <c r="S10">
-        <v>0.355</v>
+        <v>0.354</v>
       </c>
       <c r="T10">
         <v>0.352</v>
@@ -5291,16 +5291,16 @@
         <v>0.35</v>
       </c>
       <c r="W10">
-        <v>0.351</v>
+        <v>0.35</v>
       </c>
       <c r="X10">
         <v>0.002</v>
       </c>
       <c r="Y10">
-        <v>0.349</v>
+        <v>0.348</v>
       </c>
       <c r="Z10">
-        <v>0.355</v>
+        <v>0.354</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -5308,79 +5308,79 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.067</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="C11">
-        <v>0.065</v>
+        <v>0.068</v>
       </c>
       <c r="D11">
+        <v>0.076</v>
+      </c>
+      <c r="E11">
+        <v>0.062</v>
+      </c>
+      <c r="F11">
+        <v>0.064</v>
+      </c>
+      <c r="G11">
+        <v>0.037</v>
+      </c>
+      <c r="H11">
         <v>0.07199999999999999</v>
       </c>
-      <c r="E11">
-        <v>0.056</v>
-      </c>
-      <c r="F11">
+      <c r="I11">
+        <v>0.079</v>
+      </c>
+      <c r="J11">
+        <v>0.053</v>
+      </c>
+      <c r="K11">
+        <v>0.05</v>
+      </c>
+      <c r="L11">
+        <v>0.075</v>
+      </c>
+      <c r="M11">
+        <v>0.05</v>
+      </c>
+      <c r="N11">
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="O11">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="P11">
+        <v>0.066</v>
+      </c>
+      <c r="Q11">
         <v>0.059</v>
       </c>
-      <c r="G11">
-        <v>0.035</v>
-      </c>
-      <c r="H11">
-        <v>0.066</v>
-      </c>
-      <c r="I11">
-        <v>0.07199999999999999</v>
-      </c>
-      <c r="J11">
-        <v>0.049</v>
-      </c>
-      <c r="K11">
-        <v>0.049</v>
-      </c>
-      <c r="L11">
-        <v>0.06900000000000001</v>
-      </c>
-      <c r="M11">
-        <v>0.046</v>
-      </c>
-      <c r="N11">
-        <v>0.065</v>
-      </c>
-      <c r="O11">
-        <v>0.063</v>
-      </c>
-      <c r="P11">
-        <v>0.062</v>
-      </c>
-      <c r="Q11">
-        <v>0.055</v>
-      </c>
       <c r="R11">
-        <v>0.048</v>
+        <v>0.052</v>
       </c>
       <c r="S11">
-        <v>0.02</v>
+        <v>0.025</v>
       </c>
       <c r="T11">
-        <v>0.046</v>
+        <v>0.042</v>
       </c>
       <c r="U11">
+        <v>0.027</v>
+      </c>
+      <c r="V11">
+        <v>0.061</v>
+      </c>
+      <c r="W11">
+        <v>0.059</v>
+      </c>
+      <c r="X11">
+        <v>0.016</v>
+      </c>
+      <c r="Y11">
         <v>0.025</v>
       </c>
-      <c r="V11">
-        <v>0.063</v>
-      </c>
-      <c r="W11">
-        <v>0.055</v>
-      </c>
-      <c r="X11">
-        <v>0.015</v>
-      </c>
-      <c r="Y11">
-        <v>0.02</v>
-      </c>
       <c r="Z11">
-        <v>0.07199999999999999</v>
+        <v>0.079</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -5708,79 +5708,79 @@
         <v>19</v>
       </c>
       <c r="B16">
+        <v>45.631</v>
+      </c>
+      <c r="C16">
         <v>45.632</v>
       </c>
-      <c r="C16">
+      <c r="D16">
+        <v>45.624</v>
+      </c>
+      <c r="E16">
+        <v>45.637</v>
+      </c>
+      <c r="F16">
         <v>45.635</v>
       </c>
-      <c r="D16">
+      <c r="G16">
+        <v>45.66</v>
+      </c>
+      <c r="H16">
         <v>45.628</v>
       </c>
-      <c r="E16">
-        <v>45.642</v>
-      </c>
-      <c r="F16">
-        <v>45.639</v>
-      </c>
-      <c r="G16">
-        <v>45.661</v>
-      </c>
-      <c r="H16">
+      <c r="I16">
+        <v>45.622</v>
+      </c>
+      <c r="J16">
+        <v>45.645</v>
+      </c>
+      <c r="K16">
+        <v>45.648</v>
+      </c>
+      <c r="L16">
+        <v>45.625</v>
+      </c>
+      <c r="M16">
+        <v>45.648</v>
+      </c>
+      <c r="N16">
+        <v>45.629</v>
+      </c>
+      <c r="O16">
+        <v>45.63</v>
+      </c>
+      <c r="P16">
         <v>45.634</v>
       </c>
-      <c r="I16">
-        <v>45.628</v>
-      </c>
-      <c r="J16">
-        <v>45.649</v>
-      </c>
-      <c r="K16">
-        <v>45.649</v>
-      </c>
-      <c r="L16">
-        <v>45.631</v>
-      </c>
-      <c r="M16">
-        <v>45.652</v>
-      </c>
-      <c r="N16">
-        <v>45.634</v>
-      </c>
-      <c r="O16">
-        <v>45.636</v>
-      </c>
-      <c r="P16">
-        <v>45.637</v>
-      </c>
       <c r="Q16">
-        <v>45.644</v>
+        <v>45.64</v>
       </c>
       <c r="R16">
-        <v>45.649</v>
+        <v>45.646</v>
       </c>
       <c r="S16">
-        <v>45.674</v>
+        <v>45.67</v>
       </c>
       <c r="T16">
-        <v>45.651</v>
+        <v>45.655</v>
       </c>
       <c r="U16">
+        <v>45.668</v>
+      </c>
+      <c r="V16">
+        <v>45.638</v>
+      </c>
+      <c r="W16">
+        <v>45.64</v>
+      </c>
+      <c r="X16">
+        <v>0.014</v>
+      </c>
+      <c r="Y16">
+        <v>45.622</v>
+      </c>
+      <c r="Z16">
         <v>45.67</v>
-      </c>
-      <c r="V16">
-        <v>45.636</v>
-      </c>
-      <c r="W16">
-        <v>45.643</v>
-      </c>
-      <c r="X16">
-        <v>0.013</v>
-      </c>
-      <c r="Y16">
-        <v>45.628</v>
-      </c>
-      <c r="Z16">
-        <v>45.674</v>
       </c>
     </row>
     <row r="17" spans="1:26">
@@ -6588,79 +6588,79 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>3.122</v>
+        <v>3.12</v>
       </c>
       <c r="C28">
-        <v>3.125</v>
+        <v>3.121</v>
       </c>
       <c r="D28">
-        <v>3.117</v>
+        <v>3.113</v>
       </c>
       <c r="E28">
-        <v>3.133</v>
+        <v>3.128</v>
       </c>
       <c r="F28">
+        <v>3.126</v>
+      </c>
+      <c r="G28">
+        <v>3.153</v>
+      </c>
+      <c r="H28">
+        <v>3.118</v>
+      </c>
+      <c r="I28">
+        <v>3.111</v>
+      </c>
+      <c r="J28">
+        <v>3.136</v>
+      </c>
+      <c r="K28">
+        <v>3.139</v>
+      </c>
+      <c r="L28">
+        <v>3.114</v>
+      </c>
+      <c r="M28">
+        <v>3.14</v>
+      </c>
+      <c r="N28">
+        <v>3.118</v>
+      </c>
+      <c r="O28">
+        <v>3.119</v>
+      </c>
+      <c r="P28">
+        <v>3.123</v>
+      </c>
+      <c r="Q28">
         <v>3.13</v>
       </c>
-      <c r="G28">
-        <v>3.154</v>
-      </c>
-      <c r="H28">
-        <v>3.124</v>
-      </c>
-      <c r="I28">
-        <v>3.117</v>
-      </c>
-      <c r="J28">
-        <v>3.141</v>
-      </c>
-      <c r="K28">
-        <v>3.141</v>
-      </c>
-      <c r="L28">
-        <v>3.121</v>
-      </c>
-      <c r="M28">
-        <v>3.144</v>
-      </c>
-      <c r="N28">
-        <v>3.124</v>
-      </c>
-      <c r="O28">
-        <v>3.126</v>
-      </c>
-      <c r="P28">
-        <v>3.127</v>
-      </c>
-      <c r="Q28">
-        <v>3.135</v>
-      </c>
       <c r="R28">
-        <v>3.141</v>
+        <v>3.137</v>
       </c>
       <c r="S28">
-        <v>3.169</v>
+        <v>3.164</v>
       </c>
       <c r="T28">
-        <v>3.143</v>
+        <v>3.147</v>
       </c>
       <c r="U28">
-        <v>3.165</v>
+        <v>3.163</v>
       </c>
       <c r="V28">
-        <v>3.127</v>
+        <v>3.128</v>
       </c>
       <c r="W28">
-        <v>3.135</v>
+        <v>3.131</v>
       </c>
       <c r="X28">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
       <c r="Y28">
-        <v>3.117</v>
+        <v>3.111</v>
       </c>
       <c r="Z28">
-        <v>3.169</v>
+        <v>3.164</v>
       </c>
     </row>
     <row r="29" spans="1:26">
@@ -6668,79 +6668,79 @@
         <v>14</v>
       </c>
       <c r="B29">
-        <v>0.067</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="C29">
-        <v>0.065</v>
+        <v>0.068</v>
       </c>
       <c r="D29">
+        <v>0.076</v>
+      </c>
+      <c r="E29">
+        <v>0.062</v>
+      </c>
+      <c r="F29">
+        <v>0.064</v>
+      </c>
+      <c r="G29">
+        <v>0.037</v>
+      </c>
+      <c r="H29">
         <v>0.07199999999999999</v>
       </c>
-      <c r="E29">
-        <v>0.056</v>
-      </c>
-      <c r="F29">
+      <c r="I29">
+        <v>0.079</v>
+      </c>
+      <c r="J29">
+        <v>0.053</v>
+      </c>
+      <c r="K29">
+        <v>0.05</v>
+      </c>
+      <c r="L29">
+        <v>0.075</v>
+      </c>
+      <c r="M29">
+        <v>0.05</v>
+      </c>
+      <c r="N29">
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="O29">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="P29">
+        <v>0.066</v>
+      </c>
+      <c r="Q29">
         <v>0.059</v>
       </c>
-      <c r="G29">
-        <v>0.035</v>
-      </c>
-      <c r="H29">
-        <v>0.066</v>
-      </c>
-      <c r="I29">
-        <v>0.07199999999999999</v>
-      </c>
-      <c r="J29">
-        <v>0.049</v>
-      </c>
-      <c r="K29">
-        <v>0.049</v>
-      </c>
-      <c r="L29">
-        <v>0.06900000000000001</v>
-      </c>
-      <c r="M29">
-        <v>0.046</v>
-      </c>
-      <c r="N29">
-        <v>0.065</v>
-      </c>
-      <c r="O29">
-        <v>0.063</v>
-      </c>
-      <c r="P29">
-        <v>0.062</v>
-      </c>
-      <c r="Q29">
-        <v>0.055</v>
-      </c>
       <c r="R29">
-        <v>0.048</v>
+        <v>0.052</v>
       </c>
       <c r="S29">
-        <v>0.02</v>
+        <v>0.025</v>
       </c>
       <c r="T29">
-        <v>0.046</v>
+        <v>0.042</v>
       </c>
       <c r="U29">
+        <v>0.027</v>
+      </c>
+      <c r="V29">
+        <v>0.061</v>
+      </c>
+      <c r="W29">
+        <v>0.059</v>
+      </c>
+      <c r="X29">
+        <v>0.016</v>
+      </c>
+      <c r="Y29">
         <v>0.025</v>
       </c>
-      <c r="V29">
-        <v>0.063</v>
-      </c>
-      <c r="W29">
-        <v>0.055</v>
-      </c>
-      <c r="X29">
-        <v>0.015</v>
-      </c>
-      <c r="Y29">
-        <v>0.02</v>
-      </c>
       <c r="Z29">
-        <v>0.07199999999999999</v>
+        <v>0.079</v>
       </c>
     </row>
     <row r="30" spans="1:26">
@@ -7228,61 +7228,61 @@
         <v>5</v>
       </c>
       <c r="B37">
-        <v>15.926</v>
+        <v>15.927</v>
       </c>
       <c r="C37">
-        <v>15.926</v>
+        <v>15.927</v>
       </c>
       <c r="D37">
-        <v>15.928</v>
+        <v>15.929</v>
       </c>
       <c r="E37">
-        <v>15.923</v>
+        <v>15.925</v>
       </c>
       <c r="F37">
-        <v>15.924</v>
+        <v>15.925</v>
       </c>
       <c r="G37">
         <v>15.917</v>
       </c>
       <c r="H37">
-        <v>15.926</v>
+        <v>15.928</v>
       </c>
       <c r="I37">
-        <v>15.928</v>
+        <v>15.93</v>
       </c>
       <c r="J37">
-        <v>15.921</v>
+        <v>15.922</v>
       </c>
       <c r="K37">
         <v>15.921</v>
       </c>
       <c r="L37">
+        <v>15.929</v>
+      </c>
+      <c r="M37">
+        <v>15.921</v>
+      </c>
+      <c r="N37">
+        <v>15.928</v>
+      </c>
+      <c r="O37">
         <v>15.927</v>
       </c>
-      <c r="M37">
-        <v>15.92</v>
-      </c>
-      <c r="N37">
+      <c r="P37">
         <v>15.926</v>
       </c>
-      <c r="O37">
-        <v>15.925</v>
-      </c>
-      <c r="P37">
-        <v>15.925</v>
-      </c>
       <c r="Q37">
-        <v>15.923</v>
+        <v>15.924</v>
       </c>
       <c r="R37">
-        <v>15.921</v>
+        <v>15.922</v>
       </c>
       <c r="S37">
-        <v>15.912</v>
+        <v>15.914</v>
       </c>
       <c r="T37">
-        <v>15.92</v>
+        <v>15.919</v>
       </c>
       <c r="U37">
         <v>15.914</v>
@@ -7291,16 +7291,16 @@
         <v>15.925</v>
       </c>
       <c r="W37">
-        <v>15.923</v>
+        <v>15.924</v>
       </c>
       <c r="X37">
-        <v>0.004</v>
+        <v>0.005</v>
       </c>
       <c r="Y37">
-        <v>15.912</v>
+        <v>15.914</v>
       </c>
       <c r="Z37">
-        <v>15.928</v>
+        <v>15.93</v>
       </c>
     </row>
     <row r="38" spans="1:26">
@@ -7308,7 +7308,7 @@
         <v>6</v>
       </c>
       <c r="B38">
-        <v>5.892</v>
+        <v>5.893</v>
       </c>
       <c r="C38">
         <v>5.892</v>
@@ -7317,7 +7317,7 @@
         <v>5.893</v>
       </c>
       <c r="E38">
-        <v>5.891</v>
+        <v>5.892</v>
       </c>
       <c r="F38">
         <v>5.892</v>
@@ -7326,13 +7326,13 @@
         <v>5.889</v>
       </c>
       <c r="H38">
-        <v>5.892</v>
+        <v>5.893</v>
       </c>
       <c r="I38">
-        <v>5.893</v>
+        <v>5.894</v>
       </c>
       <c r="J38">
-        <v>5.89</v>
+        <v>5.891</v>
       </c>
       <c r="K38">
         <v>5.89</v>
@@ -7344,22 +7344,22 @@
         <v>5.89</v>
       </c>
       <c r="N38">
-        <v>5.892</v>
+        <v>5.893</v>
       </c>
       <c r="O38">
-        <v>5.892</v>
+        <v>5.893</v>
       </c>
       <c r="P38">
         <v>5.892</v>
       </c>
       <c r="Q38">
+        <v>5.892</v>
+      </c>
+      <c r="R38">
         <v>5.891</v>
       </c>
-      <c r="R38">
-        <v>5.89</v>
-      </c>
       <c r="S38">
-        <v>5.887</v>
+        <v>5.888</v>
       </c>
       <c r="T38">
         <v>5.89</v>
@@ -7377,10 +7377,10 @@
         <v>0.002</v>
       </c>
       <c r="Y38">
-        <v>5.887</v>
+        <v>5.888</v>
       </c>
       <c r="Z38">
-        <v>5.893</v>
+        <v>5.894</v>
       </c>
     </row>
     <row r="39" spans="1:26">
@@ -7391,13 +7391,13 @@
         <v>5.112</v>
       </c>
       <c r="C39">
-        <v>5.111</v>
+        <v>5.112</v>
       </c>
       <c r="D39">
         <v>5.112</v>
       </c>
       <c r="E39">
-        <v>5.11</v>
+        <v>5.111</v>
       </c>
       <c r="F39">
         <v>5.111</v>
@@ -7406,10 +7406,10 @@
         <v>5.108</v>
       </c>
       <c r="H39">
-        <v>5.111</v>
+        <v>5.112</v>
       </c>
       <c r="I39">
-        <v>5.112</v>
+        <v>5.113</v>
       </c>
       <c r="J39">
         <v>5.11</v>
@@ -7421,19 +7421,19 @@
         <v>5.112</v>
       </c>
       <c r="M39">
-        <v>5.109</v>
+        <v>5.11</v>
       </c>
       <c r="N39">
-        <v>5.111</v>
+        <v>5.112</v>
       </c>
       <c r="O39">
-        <v>5.111</v>
+        <v>5.112</v>
       </c>
       <c r="P39">
         <v>5.111</v>
       </c>
       <c r="Q39">
-        <v>5.11</v>
+        <v>5.111</v>
       </c>
       <c r="R39">
         <v>5.11</v>
@@ -7445,22 +7445,22 @@
         <v>5.109</v>
       </c>
       <c r="U39">
-        <v>5.107</v>
+        <v>5.108</v>
       </c>
       <c r="V39">
         <v>5.111</v>
       </c>
       <c r="W39">
-        <v>5.11</v>
+        <v>5.111</v>
       </c>
       <c r="X39">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="Y39">
         <v>5.107</v>
       </c>
       <c r="Z39">
-        <v>5.112</v>
+        <v>5.113</v>
       </c>
     </row>
     <row r="40" spans="1:26">
@@ -7474,13 +7474,13 @@
         <v>4.338</v>
       </c>
       <c r="D40">
-        <v>4.338</v>
+        <v>4.339</v>
       </c>
       <c r="E40">
         <v>4.337</v>
       </c>
       <c r="F40">
-        <v>4.337</v>
+        <v>4.338</v>
       </c>
       <c r="G40">
         <v>4.335</v>
@@ -7489,16 +7489,16 @@
         <v>4.338</v>
       </c>
       <c r="I40">
-        <v>4.338</v>
+        <v>4.339</v>
       </c>
       <c r="J40">
-        <v>4.336</v>
+        <v>4.337</v>
       </c>
       <c r="K40">
         <v>4.336</v>
       </c>
       <c r="L40">
-        <v>4.338</v>
+        <v>4.339</v>
       </c>
       <c r="M40">
         <v>4.336</v>
@@ -7510,13 +7510,13 @@
         <v>4.338</v>
       </c>
       <c r="P40">
-        <v>4.337</v>
+        <v>4.338</v>
       </c>
       <c r="Q40">
         <v>4.337</v>
       </c>
       <c r="R40">
-        <v>4.336</v>
+        <v>4.337</v>
       </c>
       <c r="S40">
         <v>4.334</v>
@@ -7525,10 +7525,10 @@
         <v>4.336</v>
       </c>
       <c r="U40">
-        <v>4.334</v>
+        <v>4.335</v>
       </c>
       <c r="V40">
-        <v>4.338</v>
+        <v>4.337</v>
       </c>
       <c r="W40">
         <v>4.337</v>
@@ -7540,7 +7540,7 @@
         <v>4.334</v>
       </c>
       <c r="Z40">
-        <v>4.338</v>
+        <v>4.339</v>
       </c>
     </row>
     <row r="41" spans="1:26">
@@ -7569,19 +7569,19 @@
         <v>2.082</v>
       </c>
       <c r="I41">
+        <v>2.083</v>
+      </c>
+      <c r="J41">
         <v>2.082</v>
       </c>
-      <c r="J41">
-        <v>2.081</v>
-      </c>
       <c r="K41">
-        <v>2.081</v>
+        <v>2.082</v>
       </c>
       <c r="L41">
         <v>2.082</v>
       </c>
       <c r="M41">
-        <v>2.081</v>
+        <v>2.082</v>
       </c>
       <c r="N41">
         <v>2.082</v>
@@ -7596,10 +7596,10 @@
         <v>2.082</v>
       </c>
       <c r="R41">
+        <v>2.082</v>
+      </c>
+      <c r="S41">
         <v>2.081</v>
-      </c>
-      <c r="S41">
-        <v>2.08</v>
       </c>
       <c r="T41">
         <v>2.081</v>
@@ -7617,10 +7617,10 @@
         <v>0.001</v>
       </c>
       <c r="Y41">
-        <v>2.08</v>
+        <v>2.081</v>
       </c>
       <c r="Z41">
-        <v>2.082</v>
+        <v>2.083</v>
       </c>
     </row>
     <row r="42" spans="1:26">
@@ -7868,79 +7868,79 @@
         <v>13</v>
       </c>
       <c r="B45">
-        <v>7.002</v>
+        <v>6.998</v>
       </c>
       <c r="C45">
-        <v>7.008</v>
+        <v>7</v>
       </c>
       <c r="D45">
+        <v>6.983</v>
+      </c>
+      <c r="E45">
+        <v>7.014</v>
+      </c>
+      <c r="F45">
+        <v>7.009</v>
+      </c>
+      <c r="G45">
+        <v>7.067</v>
+      </c>
+      <c r="H45">
         <v>6.992</v>
       </c>
-      <c r="E45">
-        <v>7.025</v>
-      </c>
-      <c r="F45">
+      <c r="I45">
+        <v>6.978</v>
+      </c>
+      <c r="J45">
+        <v>7.032</v>
+      </c>
+      <c r="K45">
+        <v>7.038</v>
+      </c>
+      <c r="L45">
+        <v>6.985</v>
+      </c>
+      <c r="M45">
+        <v>7.039</v>
+      </c>
+      <c r="N45">
+        <v>6.993</v>
+      </c>
+      <c r="O45">
+        <v>6.996</v>
+      </c>
+      <c r="P45">
+        <v>7.004</v>
+      </c>
+      <c r="Q45">
         <v>7.019</v>
       </c>
-      <c r="G45">
-        <v>7.069</v>
-      </c>
-      <c r="H45">
-        <v>7.005</v>
-      </c>
-      <c r="I45">
-        <v>6.992</v>
-      </c>
-      <c r="J45">
-        <v>7.041</v>
-      </c>
-      <c r="K45">
-        <v>7.041</v>
-      </c>
-      <c r="L45">
-        <v>6.999</v>
-      </c>
-      <c r="M45">
-        <v>7.047</v>
-      </c>
-      <c r="N45">
-        <v>7.006</v>
-      </c>
-      <c r="O45">
-        <v>7.01</v>
-      </c>
-      <c r="P45">
-        <v>7.012</v>
-      </c>
-      <c r="Q45">
-        <v>7.029</v>
-      </c>
       <c r="R45">
-        <v>7.042</v>
+        <v>7.034</v>
       </c>
       <c r="S45">
-        <v>7.101</v>
+        <v>7.09</v>
       </c>
       <c r="T45">
-        <v>7.046</v>
+        <v>7.055</v>
       </c>
       <c r="U45">
-        <v>7.091</v>
+        <v>7.087</v>
       </c>
       <c r="V45">
-        <v>7.012</v>
+        <v>7.014</v>
       </c>
       <c r="W45">
-        <v>7.028</v>
+        <v>7.02</v>
       </c>
       <c r="X45">
-        <v>0.031</v>
+        <v>0.033</v>
       </c>
       <c r="Y45">
-        <v>6.992</v>
+        <v>6.978</v>
       </c>
       <c r="Z45">
-        <v>7.101</v>
+        <v>7.09</v>
       </c>
     </row>
     <row r="46" spans="1:26">
@@ -7948,79 +7948,79 @@
         <v>14</v>
       </c>
       <c r="B46">
-        <v>0.097</v>
+        <v>0.1</v>
       </c>
       <c r="C46">
-        <v>0.093</v>
+        <v>0.098</v>
       </c>
       <c r="D46">
+        <v>0.11</v>
+      </c>
+      <c r="E46">
+        <v>0.089</v>
+      </c>
+      <c r="F46">
+        <v>0.092</v>
+      </c>
+      <c r="G46">
+        <v>0.053</v>
+      </c>
+      <c r="H46">
         <v>0.104</v>
       </c>
-      <c r="E46">
-        <v>0.081</v>
-      </c>
-      <c r="F46">
-        <v>0.08599999999999999</v>
-      </c>
-      <c r="G46">
-        <v>0.051</v>
-      </c>
-      <c r="H46">
+      <c r="I46">
+        <v>0.114</v>
+      </c>
+      <c r="J46">
+        <v>0.077</v>
+      </c>
+      <c r="K46">
+        <v>0.07199999999999999</v>
+      </c>
+      <c r="L46">
+        <v>0.109</v>
+      </c>
+      <c r="M46">
+        <v>0.07199999999999999</v>
+      </c>
+      <c r="N46">
+        <v>0.103</v>
+      </c>
+      <c r="O46">
+        <v>0.101</v>
+      </c>
+      <c r="P46">
         <v>0.095</v>
       </c>
-      <c r="I46">
-        <v>0.104</v>
-      </c>
-      <c r="J46">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="K46">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="L46">
-        <v>0.099</v>
-      </c>
-      <c r="M46">
-        <v>0.066</v>
-      </c>
-      <c r="N46">
-        <v>0.094</v>
-      </c>
-      <c r="O46">
-        <v>0.091</v>
-      </c>
-      <c r="P46">
-        <v>0.09</v>
-      </c>
       <c r="Q46">
-        <v>0.079</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="R46">
-        <v>0.07000000000000001</v>
+        <v>0.075</v>
       </c>
       <c r="S46">
-        <v>0.03</v>
+        <v>0.036</v>
       </c>
       <c r="T46">
-        <v>0.067</v>
+        <v>0.061</v>
       </c>
       <c r="U46">
+        <v>0.039</v>
+      </c>
+      <c r="V46">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="W46">
+        <v>0.08400000000000001</v>
+      </c>
+      <c r="X46">
+        <v>0.022</v>
+      </c>
+      <c r="Y46">
         <v>0.036</v>
       </c>
-      <c r="V46">
-        <v>0.09</v>
-      </c>
-      <c r="W46">
-        <v>0.079</v>
-      </c>
-      <c r="X46">
-        <v>0.021</v>
-      </c>
-      <c r="Y46">
-        <v>0.03</v>
-      </c>
       <c r="Z46">
-        <v>0.104</v>
+        <v>0.114</v>
       </c>
     </row>
     <row r="47" spans="1:26">
@@ -8372,7 +8372,7 @@
         <v>57.616</v>
       </c>
       <c r="J51">
-        <v>57.617</v>
+        <v>57.616</v>
       </c>
       <c r="K51">
         <v>57.617</v>
@@ -8396,7 +8396,7 @@
         <v>57.616</v>
       </c>
       <c r="R51">
-        <v>57.617</v>
+        <v>57.616</v>
       </c>
       <c r="S51">
         <v>57.617</v>
@@ -8411,7 +8411,7 @@
         <v>57.616</v>
       </c>
       <c r="W51">
-        <v>57.617</v>
+        <v>57.616</v>
       </c>
       <c r="X51">
         <v>0</v>
@@ -9256,16 +9256,16 @@
         <v>0.349</v>
       </c>
       <c r="F10">
-        <v>0.349</v>
+        <v>0.348</v>
       </c>
       <c r="G10">
         <v>0.352</v>
       </c>
       <c r="H10">
-        <v>0.348</v>
+        <v>0.347</v>
       </c>
       <c r="I10">
-        <v>0.347</v>
+        <v>0.346</v>
       </c>
       <c r="J10">
         <v>0.35</v>
@@ -9274,37 +9274,37 @@
         <v>0.35</v>
       </c>
       <c r="L10">
-        <v>0.348</v>
+        <v>0.347</v>
       </c>
       <c r="M10">
-        <v>0.351</v>
+        <v>0.35</v>
       </c>
       <c r="N10">
-        <v>0.348</v>
+        <v>0.347</v>
       </c>
       <c r="O10">
-        <v>0.348</v>
+        <v>0.347</v>
       </c>
       <c r="P10">
         <v>0.348</v>
       </c>
       <c r="Q10">
-        <v>0.35</v>
+        <v>0.349</v>
       </c>
       <c r="R10">
         <v>0.35</v>
       </c>
       <c r="S10">
-        <v>0.354</v>
+        <v>0.353</v>
       </c>
       <c r="T10">
         <v>0.351</v>
       </c>
       <c r="U10">
-        <v>0.354</v>
+        <v>0.353</v>
       </c>
       <c r="V10">
-        <v>0.348</v>
+        <v>0.349</v>
       </c>
       <c r="W10">
         <v>0.349</v>
@@ -9313,10 +9313,10 @@
         <v>0.002</v>
       </c>
       <c r="Y10">
-        <v>0.347</v>
+        <v>0.346</v>
       </c>
       <c r="Z10">
-        <v>0.354</v>
+        <v>0.353</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -9324,79 +9324,79 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.081</v>
+        <v>0.083</v>
       </c>
       <c r="C11">
-        <v>0.078</v>
+        <v>0.082</v>
       </c>
       <c r="D11">
+        <v>0.092</v>
+      </c>
+      <c r="E11">
+        <v>0.074</v>
+      </c>
+      <c r="F11">
+        <v>0.077</v>
+      </c>
+      <c r="G11">
+        <v>0.044</v>
+      </c>
+      <c r="H11">
         <v>0.08699999999999999</v>
       </c>
-      <c r="E11">
-        <v>0.068</v>
-      </c>
-      <c r="F11">
+      <c r="I11">
+        <v>0.095</v>
+      </c>
+      <c r="J11">
+        <v>0.064</v>
+      </c>
+      <c r="K11">
+        <v>0.061</v>
+      </c>
+      <c r="L11">
+        <v>0.091</v>
+      </c>
+      <c r="M11">
+        <v>0.06</v>
+      </c>
+      <c r="N11">
+        <v>0.08599999999999999</v>
+      </c>
+      <c r="O11">
+        <v>0.08500000000000001</v>
+      </c>
+      <c r="P11">
+        <v>0.08</v>
+      </c>
+      <c r="Q11">
         <v>0.07099999999999999</v>
       </c>
-      <c r="G11">
-        <v>0.043</v>
-      </c>
-      <c r="H11">
-        <v>0.079</v>
-      </c>
-      <c r="I11">
-        <v>0.08699999999999999</v>
-      </c>
-      <c r="J11">
-        <v>0.059</v>
-      </c>
-      <c r="K11">
-        <v>0.058</v>
-      </c>
-      <c r="L11">
-        <v>0.083</v>
-      </c>
-      <c r="M11">
-        <v>0.055</v>
-      </c>
-      <c r="N11">
-        <v>0.079</v>
-      </c>
-      <c r="O11">
-        <v>0.076</v>
-      </c>
-      <c r="P11">
-        <v>0.075</v>
-      </c>
-      <c r="Q11">
-        <v>0.066</v>
-      </c>
       <c r="R11">
-        <v>0.058</v>
+        <v>0.063</v>
       </c>
       <c r="S11">
-        <v>0.025</v>
+        <v>0.03</v>
       </c>
       <c r="T11">
-        <v>0.056</v>
+        <v>0.051</v>
       </c>
       <c r="U11">
+        <v>0.032</v>
+      </c>
+      <c r="V11">
+        <v>0.074</v>
+      </c>
+      <c r="W11">
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="X11">
+        <v>0.019</v>
+      </c>
+      <c r="Y11">
         <v>0.03</v>
       </c>
-      <c r="V11">
-        <v>0.076</v>
-      </c>
-      <c r="W11">
-        <v>0.066</v>
-      </c>
-      <c r="X11">
-        <v>0.017</v>
-      </c>
-      <c r="Y11">
-        <v>0.025</v>
-      </c>
       <c r="Z11">
-        <v>0.08699999999999999</v>
+        <v>0.095</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -9724,79 +9724,79 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>45.62</v>
+        <v>45.618</v>
       </c>
       <c r="C16">
-        <v>45.623</v>
+        <v>45.619</v>
       </c>
       <c r="D16">
+        <v>45.611</v>
+      </c>
+      <c r="E16">
+        <v>45.626</v>
+      </c>
+      <c r="F16">
+        <v>45.624</v>
+      </c>
+      <c r="G16">
+        <v>45.653</v>
+      </c>
+      <c r="H16">
         <v>45.615</v>
       </c>
-      <c r="E16">
-        <v>45.632</v>
-      </c>
-      <c r="F16">
+      <c r="I16">
+        <v>45.608</v>
+      </c>
+      <c r="J16">
+        <v>45.635</v>
+      </c>
+      <c r="K16">
+        <v>45.638</v>
+      </c>
+      <c r="L16">
+        <v>45.612</v>
+      </c>
+      <c r="M16">
+        <v>45.639</v>
+      </c>
+      <c r="N16">
+        <v>45.616</v>
+      </c>
+      <c r="O16">
+        <v>45.617</v>
+      </c>
+      <c r="P16">
+        <v>45.622</v>
+      </c>
+      <c r="Q16">
         <v>45.629</v>
       </c>
-      <c r="G16">
-        <v>45.654</v>
-      </c>
-      <c r="H16">
-        <v>45.622</v>
-      </c>
-      <c r="I16">
-        <v>45.615</v>
-      </c>
-      <c r="J16">
-        <v>45.64</v>
-      </c>
-      <c r="K16">
-        <v>45.64</v>
-      </c>
-      <c r="L16">
-        <v>45.618</v>
-      </c>
-      <c r="M16">
-        <v>45.643</v>
-      </c>
-      <c r="N16">
-        <v>45.622</v>
-      </c>
-      <c r="O16">
-        <v>45.624</v>
-      </c>
-      <c r="P16">
-        <v>45.625</v>
-      </c>
-      <c r="Q16">
-        <v>45.634</v>
-      </c>
       <c r="R16">
-        <v>45.64</v>
+        <v>45.636</v>
       </c>
       <c r="S16">
-        <v>45.67</v>
+        <v>45.665</v>
       </c>
       <c r="T16">
-        <v>45.643</v>
+        <v>45.647</v>
       </c>
       <c r="U16">
-        <v>45.666</v>
+        <v>45.663</v>
       </c>
       <c r="V16">
-        <v>45.625</v>
+        <v>45.626</v>
       </c>
       <c r="W16">
-        <v>45.633</v>
+        <v>45.629</v>
       </c>
       <c r="X16">
-        <v>0.016</v>
+        <v>0.017</v>
       </c>
       <c r="Y16">
-        <v>45.615</v>
+        <v>45.608</v>
       </c>
       <c r="Z16">
-        <v>45.67</v>
+        <v>45.665</v>
       </c>
     </row>
     <row r="17" spans="1:26">
@@ -10604,79 +10604,79 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>3.108</v>
+        <v>3.106</v>
       </c>
       <c r="C28">
-        <v>3.112</v>
+        <v>3.107</v>
       </c>
       <c r="D28">
+        <v>3.098</v>
+      </c>
+      <c r="E28">
+        <v>3.115</v>
+      </c>
+      <c r="F28">
+        <v>3.113</v>
+      </c>
+      <c r="G28">
+        <v>3.145</v>
+      </c>
+      <c r="H28">
         <v>3.103</v>
       </c>
-      <c r="E28">
-        <v>3.122</v>
-      </c>
-      <c r="F28">
+      <c r="I28">
+        <v>3.095</v>
+      </c>
+      <c r="J28">
+        <v>3.125</v>
+      </c>
+      <c r="K28">
+        <v>3.129</v>
+      </c>
+      <c r="L28">
+        <v>3.099</v>
+      </c>
+      <c r="M28">
+        <v>3.129</v>
+      </c>
+      <c r="N28">
+        <v>3.104</v>
+      </c>
+      <c r="O28">
+        <v>3.105</v>
+      </c>
+      <c r="P28">
+        <v>3.11</v>
+      </c>
+      <c r="Q28">
         <v>3.118</v>
       </c>
-      <c r="G28">
-        <v>3.147</v>
-      </c>
-      <c r="H28">
-        <v>3.11</v>
-      </c>
-      <c r="I28">
-        <v>3.103</v>
-      </c>
-      <c r="J28">
-        <v>3.131</v>
-      </c>
-      <c r="K28">
-        <v>3.131</v>
-      </c>
-      <c r="L28">
-        <v>3.107</v>
-      </c>
-      <c r="M28">
-        <v>3.134</v>
-      </c>
-      <c r="N28">
-        <v>3.111</v>
-      </c>
-      <c r="O28">
-        <v>3.113</v>
-      </c>
-      <c r="P28">
-        <v>3.114</v>
-      </c>
-      <c r="Q28">
-        <v>3.124</v>
-      </c>
       <c r="R28">
-        <v>3.131</v>
+        <v>3.127</v>
       </c>
       <c r="S28">
-        <v>3.165</v>
+        <v>3.159</v>
       </c>
       <c r="T28">
-        <v>3.134</v>
+        <v>3.139</v>
       </c>
       <c r="U28">
-        <v>3.16</v>
+        <v>3.157</v>
       </c>
       <c r="V28">
-        <v>3.114</v>
+        <v>3.116</v>
       </c>
       <c r="W28">
-        <v>3.123</v>
+        <v>3.119</v>
       </c>
       <c r="X28">
-        <v>0.017</v>
+        <v>0.019</v>
       </c>
       <c r="Y28">
-        <v>3.103</v>
+        <v>3.095</v>
       </c>
       <c r="Z28">
-        <v>3.165</v>
+        <v>3.159</v>
       </c>
     </row>
     <row r="29" spans="1:26">
@@ -10684,79 +10684,79 @@
         <v>14</v>
       </c>
       <c r="B29">
-        <v>0.081</v>
+        <v>0.083</v>
       </c>
       <c r="C29">
-        <v>0.078</v>
+        <v>0.082</v>
       </c>
       <c r="D29">
+        <v>0.092</v>
+      </c>
+      <c r="E29">
+        <v>0.074</v>
+      </c>
+      <c r="F29">
+        <v>0.077</v>
+      </c>
+      <c r="G29">
+        <v>0.044</v>
+      </c>
+      <c r="H29">
         <v>0.08699999999999999</v>
       </c>
-      <c r="E29">
-        <v>0.068</v>
-      </c>
-      <c r="F29">
+      <c r="I29">
+        <v>0.095</v>
+      </c>
+      <c r="J29">
+        <v>0.064</v>
+      </c>
+      <c r="K29">
+        <v>0.061</v>
+      </c>
+      <c r="L29">
+        <v>0.091</v>
+      </c>
+      <c r="M29">
+        <v>0.06</v>
+      </c>
+      <c r="N29">
+        <v>0.08599999999999999</v>
+      </c>
+      <c r="O29">
+        <v>0.08500000000000001</v>
+      </c>
+      <c r="P29">
+        <v>0.08</v>
+      </c>
+      <c r="Q29">
         <v>0.07099999999999999</v>
       </c>
-      <c r="G29">
-        <v>0.043</v>
-      </c>
-      <c r="H29">
-        <v>0.079</v>
-      </c>
-      <c r="I29">
-        <v>0.08699999999999999</v>
-      </c>
-      <c r="J29">
-        <v>0.059</v>
-      </c>
-      <c r="K29">
-        <v>0.058</v>
-      </c>
-      <c r="L29">
-        <v>0.083</v>
-      </c>
-      <c r="M29">
-        <v>0.055</v>
-      </c>
-      <c r="N29">
-        <v>0.079</v>
-      </c>
-      <c r="O29">
-        <v>0.076</v>
-      </c>
-      <c r="P29">
-        <v>0.075</v>
-      </c>
-      <c r="Q29">
-        <v>0.066</v>
-      </c>
       <c r="R29">
-        <v>0.058</v>
+        <v>0.063</v>
       </c>
       <c r="S29">
-        <v>0.025</v>
+        <v>0.03</v>
       </c>
       <c r="T29">
-        <v>0.056</v>
+        <v>0.051</v>
       </c>
       <c r="U29">
+        <v>0.032</v>
+      </c>
+      <c r="V29">
+        <v>0.074</v>
+      </c>
+      <c r="W29">
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="X29">
+        <v>0.019</v>
+      </c>
+      <c r="Y29">
         <v>0.03</v>
       </c>
-      <c r="V29">
-        <v>0.076</v>
-      </c>
-      <c r="W29">
-        <v>0.066</v>
-      </c>
-      <c r="X29">
-        <v>0.017</v>
-      </c>
-      <c r="Y29">
-        <v>0.025</v>
-      </c>
       <c r="Z29">
-        <v>0.08699999999999999</v>
+        <v>0.095</v>
       </c>
     </row>
     <row r="30" spans="1:26">
@@ -11247,76 +11247,76 @@
         <v>15.931</v>
       </c>
       <c r="C37">
-        <v>15.93</v>
+        <v>15.931</v>
       </c>
       <c r="D37">
-        <v>15.932</v>
+        <v>15.934</v>
       </c>
       <c r="E37">
-        <v>15.927</v>
+        <v>15.929</v>
       </c>
       <c r="F37">
-        <v>15.928</v>
+        <v>15.929</v>
       </c>
       <c r="G37">
         <v>15.919</v>
       </c>
       <c r="H37">
-        <v>15.93</v>
+        <v>15.932</v>
       </c>
       <c r="I37">
-        <v>15.932</v>
+        <v>15.935</v>
       </c>
       <c r="J37">
-        <v>15.924</v>
+        <v>15.926</v>
       </c>
       <c r="K37">
         <v>15.924</v>
       </c>
       <c r="L37">
-        <v>15.931</v>
+        <v>15.934</v>
       </c>
       <c r="M37">
-        <v>15.923</v>
+        <v>15.924</v>
       </c>
       <c r="N37">
+        <v>15.932</v>
+      </c>
+      <c r="O37">
+        <v>15.932</v>
+      </c>
+      <c r="P37">
         <v>15.93</v>
       </c>
-      <c r="O37">
-        <v>15.929</v>
-      </c>
-      <c r="P37">
-        <v>15.929</v>
-      </c>
       <c r="Q37">
-        <v>15.926</v>
+        <v>15.928</v>
       </c>
       <c r="R37">
-        <v>15.924</v>
+        <v>15.925</v>
       </c>
       <c r="S37">
-        <v>15.913</v>
+        <v>15.915</v>
       </c>
       <c r="T37">
-        <v>15.923</v>
+        <v>15.921</v>
       </c>
       <c r="U37">
-        <v>15.915</v>
+        <v>15.916</v>
       </c>
       <c r="V37">
         <v>15.929</v>
       </c>
       <c r="W37">
-        <v>15.926</v>
+        <v>15.927</v>
       </c>
       <c r="X37">
-        <v>0.005</v>
+        <v>0.006</v>
       </c>
       <c r="Y37">
-        <v>15.913</v>
+        <v>15.915</v>
       </c>
       <c r="Z37">
-        <v>15.932</v>
+        <v>15.935</v>
       </c>
     </row>
     <row r="38" spans="1:26">
@@ -11333,46 +11333,46 @@
         <v>5.895</v>
       </c>
       <c r="E38">
-        <v>5.892</v>
+        <v>5.893</v>
       </c>
       <c r="F38">
-        <v>5.893</v>
+        <v>5.894</v>
       </c>
       <c r="G38">
         <v>5.89</v>
       </c>
       <c r="H38">
-        <v>5.894</v>
+        <v>5.895</v>
       </c>
       <c r="I38">
+        <v>5.896</v>
+      </c>
+      <c r="J38">
+        <v>5.892</v>
+      </c>
+      <c r="K38">
+        <v>5.892</v>
+      </c>
+      <c r="L38">
         <v>5.895</v>
       </c>
-      <c r="J38">
-        <v>5.891</v>
-      </c>
-      <c r="K38">
-        <v>5.891</v>
-      </c>
-      <c r="L38">
-        <v>5.894</v>
-      </c>
       <c r="M38">
-        <v>5.891</v>
+        <v>5.892</v>
       </c>
       <c r="N38">
         <v>5.894</v>
       </c>
       <c r="O38">
+        <v>5.894</v>
+      </c>
+      <c r="P38">
+        <v>5.894</v>
+      </c>
+      <c r="Q38">
         <v>5.893</v>
       </c>
-      <c r="P38">
-        <v>5.893</v>
-      </c>
-      <c r="Q38">
+      <c r="R38">
         <v>5.892</v>
-      </c>
-      <c r="R38">
-        <v>5.891</v>
       </c>
       <c r="S38">
         <v>5.888</v>
@@ -11387,7 +11387,7 @@
         <v>5.893</v>
       </c>
       <c r="W38">
-        <v>5.892</v>
+        <v>5.893</v>
       </c>
       <c r="X38">
         <v>0.002</v>
@@ -11396,7 +11396,7 @@
         <v>5.888</v>
       </c>
       <c r="Z38">
-        <v>5.895</v>
+        <v>5.896</v>
       </c>
     </row>
     <row r="39" spans="1:26">
@@ -11407,10 +11407,10 @@
         <v>5.113</v>
       </c>
       <c r="C39">
-        <v>5.112</v>
+        <v>5.113</v>
       </c>
       <c r="D39">
-        <v>5.113</v>
+        <v>5.114</v>
       </c>
       <c r="E39">
         <v>5.112</v>
@@ -11425,7 +11425,7 @@
         <v>5.113</v>
       </c>
       <c r="I39">
-        <v>5.113</v>
+        <v>5.114</v>
       </c>
       <c r="J39">
         <v>5.111</v>
@@ -11434,28 +11434,28 @@
         <v>5.111</v>
       </c>
       <c r="L39">
-        <v>5.113</v>
+        <v>5.114</v>
       </c>
       <c r="M39">
-        <v>5.11</v>
+        <v>5.111</v>
       </c>
       <c r="N39">
         <v>5.113</v>
       </c>
       <c r="O39">
+        <v>5.113</v>
+      </c>
+      <c r="P39">
+        <v>5.113</v>
+      </c>
+      <c r="Q39">
         <v>5.112</v>
-      </c>
-      <c r="P39">
-        <v>5.112</v>
-      </c>
-      <c r="Q39">
-        <v>5.111</v>
       </c>
       <c r="R39">
         <v>5.111</v>
       </c>
       <c r="S39">
-        <v>5.107</v>
+        <v>5.108</v>
       </c>
       <c r="T39">
         <v>5.11</v>
@@ -11467,16 +11467,16 @@
         <v>5.112</v>
       </c>
       <c r="W39">
-        <v>5.111</v>
+        <v>5.112</v>
       </c>
       <c r="X39">
         <v>0.002</v>
       </c>
       <c r="Y39">
-        <v>5.107</v>
+        <v>5.108</v>
       </c>
       <c r="Z39">
-        <v>5.113</v>
+        <v>5.114</v>
       </c>
     </row>
     <row r="40" spans="1:26">
@@ -11496,31 +11496,31 @@
         <v>4.338</v>
       </c>
       <c r="F40">
-        <v>4.338</v>
+        <v>4.339</v>
       </c>
       <c r="G40">
         <v>4.336</v>
       </c>
       <c r="H40">
-        <v>4.339</v>
+        <v>4.34</v>
       </c>
       <c r="I40">
         <v>4.34</v>
       </c>
       <c r="J40">
-        <v>4.337</v>
+        <v>4.338</v>
       </c>
       <c r="K40">
         <v>4.337</v>
       </c>
       <c r="L40">
-        <v>4.339</v>
+        <v>4.34</v>
       </c>
       <c r="M40">
         <v>4.337</v>
       </c>
       <c r="N40">
-        <v>4.339</v>
+        <v>4.34</v>
       </c>
       <c r="O40">
         <v>4.339</v>
@@ -11532,10 +11532,10 @@
         <v>4.338</v>
       </c>
       <c r="R40">
-        <v>4.337</v>
+        <v>4.338</v>
       </c>
       <c r="S40">
-        <v>4.334</v>
+        <v>4.335</v>
       </c>
       <c r="T40">
         <v>4.337</v>
@@ -11544,16 +11544,16 @@
         <v>4.335</v>
       </c>
       <c r="V40">
-        <v>4.339</v>
+        <v>4.338</v>
       </c>
       <c r="W40">
         <v>4.338</v>
       </c>
       <c r="X40">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="Y40">
-        <v>4.334</v>
+        <v>4.335</v>
       </c>
       <c r="Z40">
         <v>4.34</v>
@@ -11603,10 +11603,10 @@
         <v>2.083</v>
       </c>
       <c r="O41">
-        <v>2.082</v>
+        <v>2.083</v>
       </c>
       <c r="P41">
-        <v>2.082</v>
+        <v>2.083</v>
       </c>
       <c r="Q41">
         <v>2.082</v>
@@ -11810,7 +11810,7 @@
         <v>1.108</v>
       </c>
       <c r="D44">
-        <v>1.108</v>
+        <v>1.109</v>
       </c>
       <c r="E44">
         <v>1.108</v>
@@ -11825,7 +11825,7 @@
         <v>1.108</v>
       </c>
       <c r="I44">
-        <v>1.108</v>
+        <v>1.109</v>
       </c>
       <c r="J44">
         <v>1.108</v>
@@ -11834,7 +11834,7 @@
         <v>1.108</v>
       </c>
       <c r="L44">
-        <v>1.108</v>
+        <v>1.109</v>
       </c>
       <c r="M44">
         <v>1.108</v>
@@ -11876,7 +11876,7 @@
         <v>1.107</v>
       </c>
       <c r="Z44">
-        <v>1.108</v>
+        <v>1.109</v>
       </c>
     </row>
     <row r="45" spans="1:26">
@@ -11884,79 +11884,79 @@
         <v>13</v>
       </c>
       <c r="B45">
-        <v>6.973</v>
+        <v>6.968</v>
       </c>
       <c r="C45">
-        <v>6.98</v>
+        <v>6.97</v>
       </c>
       <c r="D45">
+        <v>6.95</v>
+      </c>
+      <c r="E45">
+        <v>6.987</v>
+      </c>
+      <c r="F45">
+        <v>6.982</v>
+      </c>
+      <c r="G45">
+        <v>7.051</v>
+      </c>
+      <c r="H45">
         <v>6.961</v>
       </c>
-      <c r="E45">
-        <v>7.001</v>
-      </c>
-      <c r="F45">
+      <c r="I45">
+        <v>6.944</v>
+      </c>
+      <c r="J45">
+        <v>7.008</v>
+      </c>
+      <c r="K45">
+        <v>7.016</v>
+      </c>
+      <c r="L45">
+        <v>6.953</v>
+      </c>
+      <c r="M45">
+        <v>7.017</v>
+      </c>
+      <c r="N45">
+        <v>6.962</v>
+      </c>
+      <c r="O45">
+        <v>6.966</v>
+      </c>
+      <c r="P45">
+        <v>6.976</v>
+      </c>
+      <c r="Q45">
         <v>6.993</v>
       </c>
-      <c r="G45">
-        <v>7.054</v>
-      </c>
-      <c r="H45">
-        <v>6.977</v>
-      </c>
-      <c r="I45">
-        <v>6.961</v>
-      </c>
-      <c r="J45">
-        <v>7.02</v>
-      </c>
-      <c r="K45">
-        <v>7.02</v>
-      </c>
-      <c r="L45">
-        <v>6.969</v>
-      </c>
-      <c r="M45">
-        <v>7.028</v>
-      </c>
-      <c r="N45">
-        <v>6.978</v>
-      </c>
-      <c r="O45">
-        <v>6.983</v>
-      </c>
-      <c r="P45">
-        <v>6.985</v>
-      </c>
-      <c r="Q45">
-        <v>7.005</v>
-      </c>
       <c r="R45">
-        <v>7.021</v>
+        <v>7.012</v>
       </c>
       <c r="S45">
-        <v>7.092</v>
+        <v>7.079</v>
       </c>
       <c r="T45">
-        <v>7.026</v>
+        <v>7.037</v>
       </c>
       <c r="U45">
-        <v>7.081</v>
+        <v>7.075</v>
       </c>
       <c r="V45">
-        <v>6.984</v>
+        <v>6.988</v>
       </c>
       <c r="W45">
-        <v>7.004</v>
+        <v>6.995</v>
       </c>
       <c r="X45">
-        <v>0.037</v>
+        <v>0.04</v>
       </c>
       <c r="Y45">
-        <v>6.961</v>
+        <v>6.944</v>
       </c>
       <c r="Z45">
-        <v>7.092</v>
+        <v>7.079</v>
       </c>
     </row>
     <row r="46" spans="1:26">
@@ -11964,79 +11964,79 @@
         <v>14</v>
       </c>
       <c r="B46">
-        <v>0.117</v>
+        <v>0.12</v>
       </c>
       <c r="C46">
-        <v>0.112</v>
+        <v>0.119</v>
       </c>
       <c r="D46">
+        <v>0.132</v>
+      </c>
+      <c r="E46">
+        <v>0.107</v>
+      </c>
+      <c r="F46">
+        <v>0.111</v>
+      </c>
+      <c r="G46">
+        <v>0.064</v>
+      </c>
+      <c r="H46">
         <v>0.125</v>
       </c>
-      <c r="E46">
-        <v>0.098</v>
-      </c>
-      <c r="F46">
+      <c r="I46">
+        <v>0.137</v>
+      </c>
+      <c r="J46">
+        <v>0.092</v>
+      </c>
+      <c r="K46">
+        <v>0.08699999999999999</v>
+      </c>
+      <c r="L46">
+        <v>0.131</v>
+      </c>
+      <c r="M46">
+        <v>0.08699999999999999</v>
+      </c>
+      <c r="N46">
+        <v>0.124</v>
+      </c>
+      <c r="O46">
+        <v>0.122</v>
+      </c>
+      <c r="P46">
+        <v>0.115</v>
+      </c>
+      <c r="Q46">
         <v>0.103</v>
       </c>
-      <c r="G46">
-        <v>0.062</v>
-      </c>
-      <c r="H46">
-        <v>0.114</v>
-      </c>
-      <c r="I46">
-        <v>0.125</v>
-      </c>
-      <c r="J46">
-        <v>0.08400000000000001</v>
-      </c>
-      <c r="K46">
-        <v>0.08400000000000001</v>
-      </c>
-      <c r="L46">
-        <v>0.12</v>
-      </c>
-      <c r="M46">
-        <v>0.08</v>
-      </c>
-      <c r="N46">
-        <v>0.114</v>
-      </c>
-      <c r="O46">
-        <v>0.11</v>
-      </c>
-      <c r="P46">
-        <v>0.108</v>
-      </c>
-      <c r="Q46">
-        <v>0.095</v>
-      </c>
       <c r="R46">
-        <v>0.08400000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="S46">
-        <v>0.036</v>
+        <v>0.044</v>
       </c>
       <c r="T46">
-        <v>0.08</v>
+        <v>0.073</v>
       </c>
       <c r="U46">
-        <v>0.043</v>
+        <v>0.047</v>
       </c>
       <c r="V46">
-        <v>0.109</v>
+        <v>0.107</v>
       </c>
       <c r="W46">
-        <v>0.095</v>
+        <v>0.102</v>
       </c>
       <c r="X46">
-        <v>0.025</v>
+        <v>0.027</v>
       </c>
       <c r="Y46">
-        <v>0.036</v>
+        <v>0.044</v>
       </c>
       <c r="Z46">
-        <v>0.125</v>
+        <v>0.137</v>
       </c>
     </row>
     <row r="47" spans="1:26">
@@ -12142,7 +12142,7 @@
         <v>0.578</v>
       </c>
       <c r="H48">
-        <v>0.578</v>
+        <v>0.579</v>
       </c>
       <c r="I48">
         <v>0.579</v>
@@ -12154,16 +12154,16 @@
         <v>0.578</v>
       </c>
       <c r="L48">
-        <v>0.578</v>
+        <v>0.579</v>
       </c>
       <c r="M48">
         <v>0.578</v>
       </c>
       <c r="N48">
-        <v>0.578</v>
+        <v>0.579</v>
       </c>
       <c r="O48">
-        <v>0.578</v>
+        <v>0.579</v>
       </c>
       <c r="P48">
         <v>0.578</v>
@@ -12418,7 +12418,7 @@
         <v>57.617</v>
       </c>
       <c r="T51">
-        <v>57.616</v>
+        <v>57.617</v>
       </c>
       <c r="U51">
         <v>57.617</v>

</xml_diff>